<commit_message>
Sredjena stranica sa rezultatima
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="6675" windowHeight="4695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15636" windowHeight="5376"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K16"/>
 </workbook>
 </file>
 
@@ -84,7 +85,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,6 +127,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -174,7 +178,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -209,7 +213,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -421,18 +425,18 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>27</v>
       </c>
@@ -463,7 +467,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>28</v>
       </c>
@@ -480,7 +484,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>29</v>
       </c>
@@ -497,7 +501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>30</v>
       </c>
@@ -514,7 +518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>31</v>
       </c>
@@ -531,7 +535,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>32</v>
       </c>
@@ -548,7 +552,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>33</v>
       </c>
@@ -565,7 +569,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>34</v>
       </c>
@@ -582,7 +586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>35</v>
       </c>
@@ -599,7 +603,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>36</v>
       </c>
@@ -616,7 +620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>37</v>
       </c>
@@ -633,7 +637,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>38</v>
       </c>
@@ -650,7 +654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>39</v>
       </c>
@@ -667,7 +671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>40</v>
       </c>
@@ -684,7 +688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>41</v>
       </c>
@@ -701,7 +705,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>42</v>
       </c>
@@ -718,7 +722,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>43</v>
       </c>
@@ -735,7 +739,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>44</v>
       </c>
@@ -752,7 +756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>45</v>
       </c>
@@ -769,7 +773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>46</v>
       </c>
@@ -786,7 +790,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>47</v>
       </c>
@@ -803,7 +807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>48</v>
       </c>
@@ -832,7 +836,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -844,7 +848,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>